<commit_message>
Review comments about UI Design
</commit_message>
<xml_diff>
--- a/1- PM/review_sheet.xlsx
+++ b/1- PM/review_sheet.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skywa\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="55">
   <si>
     <t>review sheet</t>
   </si>
@@ -168,12 +163,45 @@
   </si>
   <si>
     <t>added track system using IDs</t>
+  </si>
+  <si>
+    <t>RV_UD_06</t>
+  </si>
+  <si>
+    <t>pages from 6 to 21</t>
+  </si>
+  <si>
+    <t>UI Design (pdf)</t>
+  </si>
+  <si>
+    <t>Abdullah</t>
+  </si>
+  <si>
+    <t>The navigation bar style needs to be edited by making its width maximum width</t>
+  </si>
+  <si>
+    <t xml:space="preserve">edited navigation bar style </t>
+  </si>
+  <si>
+    <t>20/3</t>
+  </si>
+  <si>
+    <t>RV_UD_07</t>
+  </si>
+  <si>
+    <t>Page 21</t>
+  </si>
+  <si>
+    <t>the offer name field can be a drop down list too.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">edited offer name field to be a drop down list </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -294,10 +322,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -307,12 +335,6 @@
   <dxfs count="15">
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -510,20 +532,26 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="medium">
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
+        <bottom style="medium">
           <color indexed="64"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -539,19 +567,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:J7" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="13" tableBorderDxfId="14" totalsRowBorderDxfId="12">
-  <autoFilter ref="A2:J7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:J9" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11" totalsRowBorderDxfId="10">
+  <autoFilter ref="A2:J9"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="id " dataDxfId="11"/>
-    <tableColumn id="2" name="filename" dataDxfId="10"/>
-    <tableColumn id="3" name="section " dataDxfId="9"/>
-    <tableColumn id="4" name="revierwer " dataDxfId="8"/>
-    <tableColumn id="5" name="finding " dataDxfId="7"/>
-    <tableColumn id="6" name="action " dataDxfId="6"/>
-    <tableColumn id="7" name="owner" dataDxfId="5"/>
-    <tableColumn id="8" name="intial date" dataDxfId="4"/>
-    <tableColumn id="9" name="status" dataDxfId="3"/>
-    <tableColumn id="10" name="cloing date " dataDxfId="2"/>
+    <tableColumn id="1" name="id " dataDxfId="9"/>
+    <tableColumn id="2" name="filename" dataDxfId="8"/>
+    <tableColumn id="3" name="section " dataDxfId="7"/>
+    <tableColumn id="4" name="revierwer " dataDxfId="6"/>
+    <tableColumn id="5" name="finding " dataDxfId="5"/>
+    <tableColumn id="6" name="action " dataDxfId="4"/>
+    <tableColumn id="7" name="owner" dataDxfId="3"/>
+    <tableColumn id="8" name="intial date" dataDxfId="2"/>
+    <tableColumn id="9" name="status" dataDxfId="1"/>
+    <tableColumn id="10" name="cloing date " dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -600,7 +628,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -652,7 +680,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -846,7 +874,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -856,8 +884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -875,18 +903,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="61.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
@@ -1049,60 +1077,100 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="J7" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
+      <c r="A8" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="9" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="A9" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="10" spans="1:10" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>

</xml_diff>